<commit_message>
"#55: fixed import and timeslot management"
</commit_message>
<xml_diff>
--- a/src/test/resources/IMPORT BOT0_Raumliste.xlsx
+++ b/src/test/resources/IMPORT BOT0_Raumliste.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20394"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\+++Schule\AE_LF12\Projekt Berufsorientierungstag\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\Documents\AE_LF12\Projekt Berufsorientierungstag\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{77A99E5A-1480-4E7E-9627-7C0EA70C4D0A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD785030-4060-4B7A-B7F1-6E5957A06EE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{254B5C5A-C805-468E-BF4E-A3CDD66F8374}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{254B5C5A-C805-468E-BF4E-A3CDD66F8374}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,12 +25,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>008</t>
   </si>
   <si>
     <t>Aula</t>
+  </si>
+  <si>
+    <t>Raum</t>
+  </si>
+  <si>
+    <t>Kapazität</t>
   </si>
 </sst>
 </file>
@@ -66,7 +72,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
@@ -383,82 +390,132 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C0EFAA5-628D-4D52-9815-787F64D78A8F}">
-  <dimension ref="A1:A14"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="A16" sqref="A16:XFD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="B2" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
         <v>101</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="B3" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
         <v>102</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="B4" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
         <v>103</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="B5" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
         <v>106</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="B6" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
         <v>107</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="B7" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
         <v>108</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="B8" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
         <v>109</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="B9" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
         <v>110</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="B10" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
         <v>111</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11">
+      <c r="B11" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
         <v>112</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12">
+      <c r="B12" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
         <v>113</v>
       </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="B13" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14">
+      <c r="B14" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
         <v>209</v>
+      </c>
+      <c r="B15" s="1">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>